<commit_message>
descriptive stats including elevated lead
</commit_message>
<xml_diff>
--- a/school-stats.xlsx
+++ b/school-stats.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/misbath/Desktop/Analytical Mthds EHS/aamehs_group/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F979E09-674F-1948-9E77-E533B04F3554}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF4FB9B1-C3D8-AD4F-89C6-34F2ED14A3CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="39840" yWindow="6420" windowWidth="28040" windowHeight="16660" xr2:uid="{DE9B9CD3-72C9-F446-A5C0-EA4422DE0938}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>n</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>% Multiple race categories not represented</t>
+  </si>
+  <si>
+    <t xml:space="preserve">% Elevated </t>
   </si>
 </sst>
 </file>
@@ -120,7 +123,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -262,22 +265,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -315,6 +324,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -629,10 +656,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F90719ED-EFB9-1F4F-9390-1F0A955D109B}">
-  <dimension ref="B2:N14"/>
+  <dimension ref="B2:N15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:N14"/>
+      <selection activeCell="B2" sqref="B2:N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -642,511 +669,552 @@
   <sheetData>
     <row r="2" spans="2:14" ht="18">
       <c r="B2" s="1"/>
-      <c r="C2" s="2">
+      <c r="C2" s="15">
         <v>2016</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="2">
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="15">
         <v>2017</v>
       </c>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="4"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="17"/>
     </row>
     <row r="3" spans="2:14" ht="18">
-      <c r="B3" s="17"/>
-      <c r="C3" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="6" t="s">
+      <c r="B3" s="14"/>
+      <c r="C3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="J3" s="6" t="s">
+      <c r="I3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="L3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="M3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="7" t="s">
+      <c r="N3" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="2:14" ht="19">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="7">
         <v>1027</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="8">
         <v>49.02</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4" s="8">
         <v>6.26</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="8">
         <v>48.8</v>
       </c>
-      <c r="G4" s="11">
-        <v>0</v>
-      </c>
-      <c r="H4" s="12">
+      <c r="G4" s="8">
+        <v>0</v>
+      </c>
+      <c r="H4" s="9">
         <v>100</v>
       </c>
-      <c r="I4" s="10">
+      <c r="I4" s="7">
         <v>1037</v>
       </c>
-      <c r="J4" s="11">
+      <c r="J4" s="8">
         <v>49.01</v>
       </c>
-      <c r="K4" s="11">
+      <c r="K4" s="8">
         <v>6.24</v>
       </c>
-      <c r="L4" s="11">
+      <c r="L4" s="8">
         <v>48.8</v>
       </c>
-      <c r="M4" s="11">
-        <v>0</v>
-      </c>
-      <c r="N4" s="12">
+      <c r="M4" s="8">
+        <v>0</v>
+      </c>
+      <c r="N4" s="9">
         <v>100</v>
       </c>
     </row>
     <row r="5" spans="2:14" ht="19">
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="7">
         <v>1027</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="8">
         <v>50.98</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5" s="8">
         <v>6.26</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="8">
         <v>51.2</v>
       </c>
-      <c r="G5" s="11">
-        <v>0</v>
-      </c>
-      <c r="H5" s="12">
+      <c r="G5" s="8">
+        <v>0</v>
+      </c>
+      <c r="H5" s="9">
         <v>100</v>
       </c>
-      <c r="I5" s="10">
+      <c r="I5" s="7">
         <v>1037</v>
       </c>
-      <c r="J5" s="11">
+      <c r="J5" s="8">
         <v>50.99</v>
       </c>
-      <c r="K5" s="11">
+      <c r="K5" s="8">
         <v>6.24</v>
       </c>
-      <c r="L5" s="11">
+      <c r="L5" s="8">
         <v>51.2</v>
       </c>
-      <c r="M5" s="11">
-        <v>0</v>
-      </c>
-      <c r="N5" s="12">
+      <c r="M5" s="8">
+        <v>0</v>
+      </c>
+      <c r="N5" s="9">
         <v>100</v>
       </c>
     </row>
     <row r="6" spans="2:14" ht="19">
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="7">
         <v>1027</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="8">
         <v>13.56</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6" s="8">
         <v>18.82</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="8">
         <v>4.5999999999999996</v>
       </c>
-      <c r="G6" s="11">
-        <v>0</v>
-      </c>
-      <c r="H6" s="12">
+      <c r="G6" s="8">
+        <v>0</v>
+      </c>
+      <c r="H6" s="9">
         <v>94.4</v>
       </c>
-      <c r="I6" s="10">
+      <c r="I6" s="7">
         <v>1037</v>
       </c>
-      <c r="J6" s="11">
+      <c r="J6" s="8">
         <v>13.51</v>
       </c>
-      <c r="K6" s="11">
+      <c r="K6" s="8">
         <v>18.760000000000002</v>
       </c>
-      <c r="L6" s="11">
+      <c r="L6" s="8">
         <v>4.5999999999999996</v>
       </c>
-      <c r="M6" s="11">
-        <v>0</v>
-      </c>
-      <c r="N6" s="12">
+      <c r="M6" s="8">
+        <v>0</v>
+      </c>
+      <c r="N6" s="9">
         <v>94.4</v>
       </c>
     </row>
     <row r="7" spans="2:14" ht="19">
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="7">
         <v>1027</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="8">
         <v>27.85</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="8">
         <v>27.27</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="8">
         <v>18.5</v>
       </c>
-      <c r="G7" s="11">
-        <v>0</v>
-      </c>
-      <c r="H7" s="12">
+      <c r="G7" s="8">
+        <v>0</v>
+      </c>
+      <c r="H7" s="9">
         <v>96.3</v>
       </c>
-      <c r="I7" s="10">
+      <c r="I7" s="7">
         <v>1037</v>
       </c>
-      <c r="J7" s="11">
+      <c r="J7" s="8">
         <v>27.68</v>
       </c>
-      <c r="K7" s="11">
+      <c r="K7" s="8">
         <v>27.21</v>
       </c>
-      <c r="L7" s="11">
+      <c r="L7" s="8">
         <v>18.100000000000001</v>
       </c>
-      <c r="M7" s="11">
-        <v>0</v>
-      </c>
-      <c r="N7" s="12">
+      <c r="M7" s="8">
+        <v>0</v>
+      </c>
+      <c r="N7" s="9">
         <v>96.3</v>
       </c>
     </row>
     <row r="8" spans="2:14" ht="19">
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="7">
         <v>1027</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="8">
         <v>41.4</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8" s="8">
         <v>26.38</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="8">
         <v>34.799999999999997</v>
       </c>
-      <c r="G8" s="11">
+      <c r="G8" s="8">
         <v>1.5</v>
       </c>
-      <c r="H8" s="12">
+      <c r="H8" s="9">
         <v>99.4</v>
       </c>
-      <c r="I8" s="10">
+      <c r="I8" s="7">
         <v>1037</v>
       </c>
-      <c r="J8" s="11">
+      <c r="J8" s="8">
         <v>41.54</v>
       </c>
-      <c r="K8" s="11">
+      <c r="K8" s="8">
         <v>26.43</v>
       </c>
-      <c r="L8" s="11">
+      <c r="L8" s="8">
         <v>35.1</v>
       </c>
-      <c r="M8" s="11">
+      <c r="M8" s="8">
         <v>1.5</v>
       </c>
-      <c r="N8" s="12">
+      <c r="N8" s="9">
         <v>99.4</v>
       </c>
     </row>
     <row r="9" spans="2:14" ht="19">
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="7">
         <v>1027</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="8">
         <v>14.86</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E9" s="8">
         <v>20.92</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="8">
         <v>3.5</v>
       </c>
-      <c r="G9" s="11">
-        <v>0</v>
-      </c>
-      <c r="H9" s="12">
+      <c r="G9" s="8">
+        <v>0</v>
+      </c>
+      <c r="H9" s="9">
         <v>93.3</v>
       </c>
-      <c r="I9" s="10">
+      <c r="I9" s="7">
         <v>1037</v>
       </c>
-      <c r="J9" s="11">
+      <c r="J9" s="8">
         <v>14.93</v>
       </c>
-      <c r="K9" s="11">
+      <c r="K9" s="8">
         <v>20.92</v>
       </c>
-      <c r="L9" s="11">
+      <c r="L9" s="8">
         <v>3.6</v>
       </c>
-      <c r="M9" s="11">
-        <v>0</v>
-      </c>
-      <c r="N9" s="12">
+      <c r="M9" s="8">
+        <v>0</v>
+      </c>
+      <c r="N9" s="9">
         <v>93.3</v>
       </c>
     </row>
     <row r="10" spans="2:14" ht="38">
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="7">
         <v>1027</v>
       </c>
-      <c r="D10" s="11">
+      <c r="D10" s="8">
         <v>2.33</v>
       </c>
-      <c r="E10" s="11">
+      <c r="E10" s="8">
         <v>2.74</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="8">
         <v>1.5</v>
       </c>
-      <c r="G10" s="11">
-        <v>0</v>
-      </c>
-      <c r="H10" s="12">
+      <c r="G10" s="8">
+        <v>0</v>
+      </c>
+      <c r="H10" s="9">
         <v>25.3</v>
       </c>
-      <c r="I10" s="10">
+      <c r="I10" s="7">
         <v>1037</v>
       </c>
-      <c r="J10" s="11">
+      <c r="J10" s="8">
         <v>2.33</v>
       </c>
-      <c r="K10" s="11">
+      <c r="K10" s="8">
         <v>2.75</v>
       </c>
-      <c r="L10" s="11">
+      <c r="L10" s="8">
         <v>1.5</v>
       </c>
-      <c r="M10" s="11">
-        <v>0</v>
-      </c>
-      <c r="N10" s="12">
+      <c r="M10" s="8">
+        <v>0</v>
+      </c>
+      <c r="N10" s="9">
         <v>25.3</v>
       </c>
     </row>
     <row r="11" spans="2:14" ht="19">
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="7">
         <v>1027</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="8">
         <v>21.12</v>
       </c>
-      <c r="E11" s="11">
+      <c r="E11" s="8">
         <v>6.56</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="8">
         <v>20.7</v>
       </c>
-      <c r="G11" s="11">
-        <v>0</v>
-      </c>
-      <c r="H11" s="12">
+      <c r="G11" s="8">
+        <v>0</v>
+      </c>
+      <c r="H11" s="9">
         <v>46.6</v>
       </c>
-      <c r="I11" s="10">
+      <c r="I11" s="7">
         <v>1037</v>
       </c>
-      <c r="J11" s="11">
+      <c r="J11" s="8">
         <v>21.12</v>
       </c>
-      <c r="K11" s="11">
+      <c r="K11" s="8">
         <v>6.55</v>
       </c>
-      <c r="L11" s="11">
+      <c r="L11" s="8">
         <v>20.7</v>
       </c>
-      <c r="M11" s="11">
-        <v>0</v>
-      </c>
-      <c r="N11" s="12">
+      <c r="M11" s="8">
+        <v>0</v>
+      </c>
+      <c r="N11" s="9">
         <v>46.6</v>
       </c>
     </row>
     <row r="12" spans="2:14" ht="19" customHeight="1">
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="7">
         <v>1027</v>
       </c>
-      <c r="D12" s="11">
+      <c r="D12" s="8">
         <v>14.23</v>
       </c>
-      <c r="E12" s="11">
+      <c r="E12" s="8">
         <v>12.08</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F12" s="8">
         <v>11.1</v>
       </c>
-      <c r="G12" s="11">
-        <v>0</v>
-      </c>
-      <c r="H12" s="12">
+      <c r="G12" s="8">
+        <v>0</v>
+      </c>
+      <c r="H12" s="9">
         <v>99.3</v>
       </c>
-      <c r="I12" s="10">
+      <c r="I12" s="7">
         <v>1037</v>
       </c>
-      <c r="J12" s="11">
+      <c r="J12" s="8">
         <v>14.35</v>
       </c>
-      <c r="K12" s="11">
+      <c r="K12" s="8">
         <v>12.26</v>
       </c>
-      <c r="L12" s="11">
+      <c r="L12" s="8">
         <v>11.2</v>
       </c>
-      <c r="M12" s="11">
-        <v>0</v>
-      </c>
-      <c r="N12" s="12">
+      <c r="M12" s="8">
+        <v>0</v>
+      </c>
+      <c r="N12" s="9">
         <v>99.3</v>
       </c>
     </row>
     <row r="13" spans="2:14" ht="19">
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="7">
         <v>1027</v>
       </c>
-      <c r="D13" s="11">
+      <c r="D13" s="8">
         <v>72.89</v>
       </c>
-      <c r="E13" s="11">
+      <c r="E13" s="8">
         <v>22.89</v>
       </c>
-      <c r="F13" s="11">
+      <c r="F13" s="8">
         <v>79.400000000000006</v>
       </c>
-      <c r="G13" s="11">
+      <c r="G13" s="8">
         <v>2.9</v>
       </c>
-      <c r="H13" s="12">
+      <c r="H13" s="9">
         <v>100</v>
       </c>
-      <c r="I13" s="10">
+      <c r="I13" s="7">
         <v>1037</v>
       </c>
-      <c r="J13" s="11">
+      <c r="J13" s="8">
         <v>72.790000000000006</v>
       </c>
-      <c r="K13" s="11">
+      <c r="K13" s="8">
         <v>22.98</v>
       </c>
-      <c r="L13" s="11">
+      <c r="L13" s="8">
         <v>79.3</v>
       </c>
-      <c r="M13" s="11">
+      <c r="M13" s="8">
         <v>2.9</v>
       </c>
-      <c r="N13" s="12">
+      <c r="N13" s="9">
         <v>100</v>
       </c>
     </row>
     <row r="14" spans="2:14" ht="19">
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="14">
+      <c r="C14" s="11">
         <v>1027</v>
       </c>
-      <c r="D14" s="15">
+      <c r="D14" s="12">
         <v>62.93</v>
       </c>
-      <c r="E14" s="15">
+      <c r="E14" s="12">
         <v>22.88</v>
       </c>
-      <c r="F14" s="15">
+      <c r="F14" s="12">
         <v>68</v>
       </c>
-      <c r="G14" s="15">
+      <c r="G14" s="12">
         <v>3</v>
       </c>
-      <c r="H14" s="16">
+      <c r="H14" s="13">
         <v>95.4</v>
       </c>
-      <c r="I14" s="14">
+      <c r="I14" s="11">
         <v>1037</v>
       </c>
-      <c r="J14" s="15">
+      <c r="J14" s="12">
         <v>62.82</v>
       </c>
-      <c r="K14" s="15">
+      <c r="K14" s="12">
         <v>22.89</v>
       </c>
-      <c r="L14" s="15">
+      <c r="L14" s="12">
         <v>67.900000000000006</v>
       </c>
-      <c r="M14" s="15">
+      <c r="M14" s="12">
         <v>3</v>
       </c>
-      <c r="N14" s="16">
+      <c r="N14" s="13">
         <v>95.4</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" ht="19">
+      <c r="B15" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="18">
+        <v>1027</v>
+      </c>
+      <c r="D15" s="18">
+        <v>0.08</v>
+      </c>
+      <c r="E15" s="18">
+        <v>0.06</v>
+      </c>
+      <c r="F15" s="18">
+        <v>0.06</v>
+      </c>
+      <c r="G15" s="18">
+        <v>0</v>
+      </c>
+      <c r="H15" s="19">
+        <v>0.39</v>
+      </c>
+      <c r="I15" s="18">
+        <v>1037</v>
+      </c>
+      <c r="J15" s="18">
+        <v>0.08</v>
+      </c>
+      <c r="K15" s="18">
+        <v>0.06</v>
+      </c>
+      <c r="L15" s="18">
+        <v>0.06</v>
+      </c>
+      <c r="M15" s="18">
+        <v>0</v>
+      </c>
+      <c r="N15" s="19">
+        <v>0.39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>